<commit_message>
evento atualizar estado + fix pout-pourri
</commit_message>
<xml_diff>
--- a/cadastro_melomano/temp.xlsx
+++ b/cadastro_melomano/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,7 +499,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Deep Purple In Rock</t>
+          <t>Deep Purple In Rock (1970)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Harvest – SHVL 777, Harvest – 1E 062 º 91442</t>
+          <t>Harvest - SHVL 777, Harvest - 1E 062 º 91442</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -521,21 +521,264 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Speed King
- / Bloodsucker
- / Child In Time
- / Flight Of The Rat
- / Into The Fire
- / Living Wreck
- / Hard Lovin' Man</t>
+          <t>Speed King / Bloodsucker / Child In Time / Flight Of The Rat / Into The Fire / Living Wreck / Hard Lovin' Man</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Progressive - Electronic - Psych - Folk</t>
+          <t>Escolha o estilo</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>aksdjfbksdfbs</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>açsndalçjkdbna</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>sçdjnsdf</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Speed King / Bloodsucker / Child In Time / Flight Of The Rat / Into The Fire / Living Wreck / Hard Lovin' Man</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Escolha o estilo</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>